<commit_message>
Added rows API to push the data to table
</commit_message>
<xml_diff>
--- a/coinalyze_data.xlsx
+++ b/coinalyze_data.xlsx
@@ -497,16 +497,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>22972321189.26739</v>
+        <v>22950771235.97675</v>
       </c>
       <c r="D3" t="n">
-        <v>24397468079.37269</v>
+        <v>24375759418.22945</v>
       </c>
       <c r="E3" t="n">
-        <v>89585.25999999999</v>
+        <v>89718.73</v>
       </c>
       <c r="F3" t="n">
-        <v>89513.89999999999</v>
+        <v>89675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>